<commit_message>
En update in Excelfile
</commit_message>
<xml_diff>
--- a/doc/JML en Javadoc.xlsx
+++ b/doc/JML en Javadoc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>CLASS</t>
   </si>
@@ -457,7 +457,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +533,9 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
MinMaxStrategy en Strategy JML/Javadoc
</commit_message>
<xml_diff>
--- a/doc/JML en Javadoc.xlsx
+++ b/doc/JML en Javadoc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>CLASS</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>CHECK</t>
+  </si>
+  <si>
+    <t>LOOPINVARIANT</t>
+  </si>
+  <si>
+    <t>PRIVATE INVARIANT</t>
   </si>
 </sst>
 </file>
@@ -460,12 +466,14 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -478,6 +486,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
@@ -674,6 +688,12 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>